<commit_message>
Basic formula suport for MS Excel
</commit_message>
<xml_diff>
--- a/demo/demo_ms_excel.xlsx
+++ b/demo/demo_ms_excel.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\opentbs\demo\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="45" windowWidth="17400" windowHeight="11955" activeTab="1"/>
   </bookViews>
@@ -15,7 +20,7 @@
   <definedNames>
     <definedName name="the_named_cell">'Delete me'!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -25,7 +30,7 @@
     <author>Qwerty</author>
   </authors>
   <commentList>
-    <comment ref="F18" authorId="0">
+    <comment ref="F18" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -51,7 +56,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E21" authorId="0">
+    <comment ref="E21" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -81,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>PHP version : [onshow..cst.PHP_VERSION]</t>
   </si>
@@ -330,11 +335,20 @@
   <si>
     <t>Score again</t>
   </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>tbs:f</t>
+  </si>
+  <si>
+    <t>[onshow.x_formula;ope=tbs:f]</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     <numFmt numFmtId="165" formatCode="dd\ mmmm\ yyyy"/>
@@ -492,7 +506,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -521,10 +535,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Titre 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Nadpis 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -537,14 +552,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="fr-FR"/>
+  <c:lang val="sk-SK"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -587,7 +605,7 @@
             <c:numRef>
               <c:f>'Examples part 1'!$E$20:$E$23</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.0</c:formatCode>
+                <c:formatCode>#\ ##0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -598,6 +616,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F19D-4495-A8D7-2F2550CDCEEF}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -618,6 +641,7 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -636,7 +660,7 @@
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="#,##0.0" sourceLinked="1"/>
+        <c:numFmt formatCode="#\ ##0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -678,7 +702,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Graphique 1"/>
+        <xdr:cNvPr id="2" name="Graphique 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -713,7 +743,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="[onshow.x_picture;ope=changepic;tagpos=inside;adjust=inside;unique]"/>
+        <xdr:cNvPr id="2" name="Image 1" descr="[onshow.x_picture;ope=changepic;tagpos=inside;adjust=inside;unique]">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -746,7 +782,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motív balíka Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -788,7 +824,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -821,9 +857,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -856,6 +909,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1032,11 +1102,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H36"/>
+  <dimension ref="B2:H37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
@@ -1159,7 +1231,7 @@
         <v>35</v>
       </c>
       <c r="E21" s="15">
-        <f ca="1">SUM( E20           : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
+        <f ca="1">SUM( E20             : INDIRECT(ADDRESS(ROW()-1,COLUMN())) )</f>
         <v>0</v>
       </c>
     </row>
@@ -1241,6 +1313,17 @@
       </c>
       <c r="D36" s="7" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="18" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1341,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.140625" customWidth="1"/>
     <col min="4" max="6" width="20.7109375" customWidth="1"/>
@@ -1348,7 +1431,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -1366,7 +1449,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="2:2" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B2" s="17" t="s">

</xml_diff>